<commit_message>
MODULO CITAS EN CLIENTES YA ESTA, COMENZANDO EDITAR Y ELIMINAR
</commit_message>
<xml_diff>
--- a/assets/PFPL01 - Lista de chequeo producto software.xlsx
+++ b/assets/PFPL01 - Lista de chequeo producto software.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIENTE 314\Downloads\DOCUMENTACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\APP-WEB-SENA-2\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9004BC-D4FB-4F81-8C5E-86E5A0F063DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9A46BA-5D98-4BC7-851E-B81B078CF6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="772" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -30,12 +30,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -360,87 +371,6 @@
   </si>
   <si>
     <t>SGCitas</t>
-  </si>
-  <si>
-    <t>Registro</t>
-  </si>
-  <si>
-    <t>Definir si se trata de un estilista o un cliente</t>
-  </si>
-  <si>
-    <t>Llenar formulario de registro</t>
-  </si>
-  <si>
-    <t>Validar captcha</t>
-  </si>
-  <si>
-    <t>Ingresar datos de inicio</t>
-  </si>
-  <si>
-    <t>Cambiar contraseña</t>
-  </si>
-  <si>
-    <t>Ingresar correo para confirmacion</t>
-  </si>
-  <si>
-    <t>Crear nomina</t>
-  </si>
-  <si>
-    <t>Actualizar nomina</t>
-  </si>
-  <si>
-    <t>Consultar nomina</t>
-  </si>
-  <si>
-    <t>Borrar nomina</t>
-  </si>
-  <si>
-    <t>Ingresar mes deseado</t>
-  </si>
-  <si>
-    <t>Iniciar sesion</t>
-  </si>
-  <si>
-    <t>Ingresar datos del trabajador</t>
-  </si>
-  <si>
-    <t>Ingreasr dias laborados del mes</t>
-  </si>
-  <si>
-    <t>Agendar cita/Seleccionar fecha y hora</t>
-  </si>
-  <si>
-    <t>Selección servicio</t>
-  </si>
-  <si>
-    <t>Seleccionar estilista</t>
-  </si>
-  <si>
-    <t>ID de la cita</t>
-  </si>
-  <si>
-    <t>Modificar cita</t>
-  </si>
-  <si>
-    <t>Cancelar cita</t>
-  </si>
-  <si>
-    <t>Crear producto</t>
-  </si>
-  <si>
-    <t>Ingresar nombre del producto</t>
-  </si>
-  <si>
-    <t>Consultar producto</t>
-  </si>
-  <si>
-    <t>Ingresar cantidad de unidades</t>
-  </si>
-  <si>
-    <t>Actualizar inventario</t>
-  </si>
-  <si>
-    <t>Eliminar producto</t>
   </si>
   <si>
     <t>USUARIO</t>
@@ -1337,6 +1267,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1355,7 +1338,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1375,64 +1357,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2" xr:uid="{1EB9EC41-D830-4ACE-B66C-36C057A1DC02}"/>
@@ -1825,91 +1755,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickTop="1">
       <c r="F6" s="10"/>
     </row>
     <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.75" thickTop="1">
       <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="70"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="63"/>
     </row>
     <row r="13" spans="2:6" ht="18.75" thickBot="1">
       <c r="B13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="70"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="63"/>
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="72"/>
+      <c r="D14" s="65"/>
       <c r="E14" s="13" t="s">
         <v>23</v>
       </c>
@@ -1921,10 +1851,10 @@
       <c r="B15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="74"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="15" t="s">
         <v>27</v>
       </c>
@@ -1936,10 +1866,10 @@
       <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="76"/>
+      <c r="D16" s="69"/>
       <c r="E16" s="17" t="s">
         <v>30</v>
       </c>
@@ -1949,8 +1879,8 @@
     </row>
     <row r="17" spans="2:16" ht="17.25" thickTop="1">
       <c r="B17" s="19"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -1969,10 +1899,10 @@
       <c r="C21" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="66" t="s">
+      <c r="D21" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="66"/>
+      <c r="E21" s="71"/>
       <c r="F21" s="24" t="s">
         <v>36</v>
       </c>
@@ -1984,10 +1914,10 @@
       <c r="C22" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="67"/>
+      <c r="E22" s="72"/>
       <c r="F22" s="27" t="s">
         <v>24</v>
       </c>
@@ -1995,57 +1925,57 @@
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="30"/>
     </row>
     <row r="24" spans="2:16" ht="25.5" customHeight="1">
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
       <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -2056,51 +1986,51 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="62"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="82"/>
     </row>
     <row r="35" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="63"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="65"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="85"/>
     </row>
     <row r="36" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="52"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="54"/>
+      <c r="B36" s="73"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="75"/>
       <c r="J36" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="75"/>
     </row>
     <row r="38" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="75"/>
     </row>
     <row r="39" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="78"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="34"/>
@@ -2261,12 +2191,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
@@ -2279,16 +2213,12 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2301,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2318,7 +2248,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="C1" s="41"/>
       <c r="D1" s="42"/>
@@ -2341,9 +2271,7 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>108</v>
-      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="str">
         <f>IF(C3="Cumple","Ninguna","")</f>
@@ -2354,9 +2282,7 @@
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="87" t="s">
-        <v>109</v>
-      </c>
+      <c r="B4" s="52"/>
       <c r="C4" s="5"/>
       <c r="D4" s="6" t="str">
         <f t="shared" ref="D4:D16" si="0">IF(C4="Cumple","Ninguna","")</f>
@@ -2367,9 +2293,7 @@
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="87" t="s">
-        <v>110</v>
-      </c>
+      <c r="B5" s="52"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2380,9 +2304,7 @@
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="87" t="s">
-        <v>111</v>
-      </c>
+      <c r="B6" s="52"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2393,9 +2315,7 @@
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2406,9 +2326,7 @@
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2419,9 +2337,7 @@
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2432,9 +2348,7 @@
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2445,9 +2359,7 @@
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2458,9 +2370,7 @@
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>121</v>
-      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2471,9 +2381,7 @@
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="B13" s="6"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2484,9 +2392,7 @@
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>122</v>
-      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2497,9 +2403,7 @@
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2510,9 +2414,7 @@
       <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>118</v>
-      </c>
+      <c r="B16" s="6"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2523,9 +2425,7 @@
       <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>119</v>
-      </c>
+      <c r="B17" s="6"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
     </row>
@@ -2533,9 +2433,7 @@
       <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>123</v>
-      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
     </row>
@@ -2543,9 +2441,7 @@
       <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>124</v>
-      </c>
+      <c r="B19" s="6"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
     </row>
@@ -2553,9 +2449,7 @@
       <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>125</v>
-      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
     </row>
@@ -2563,9 +2457,7 @@
       <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>126</v>
-      </c>
+      <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
     </row>
@@ -2573,9 +2465,7 @@
       <c r="A22" s="8">
         <v>20</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>127</v>
-      </c>
+      <c r="B22" s="6"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
     </row>
@@ -2583,9 +2473,7 @@
       <c r="A23" s="8">
         <v>21</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
     </row>
@@ -2593,9 +2481,7 @@
       <c r="A24" s="8">
         <v>22</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="B24" s="6"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
     </row>
@@ -2603,9 +2489,7 @@
       <c r="A25" s="8">
         <v>23</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="B25" s="6"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
     </row>
@@ -2613,9 +2497,7 @@
       <c r="A26" s="8">
         <v>24</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="B26" s="6"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
     </row>
@@ -2623,9 +2505,7 @@
       <c r="A27" s="8">
         <v>25</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>131</v>
-      </c>
+      <c r="B27" s="6"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
     </row>
@@ -2633,9 +2513,7 @@
       <c r="A28" s="8">
         <v>26</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="B28" s="6"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
     </row>
@@ -2643,9 +2521,7 @@
       <c r="A29" s="8">
         <v>27</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>134</v>
-      </c>
+      <c r="B29" s="6"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
     </row>
@@ -2654,7 +2530,7 @@
         <v>48</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="C30" s="41"/>
       <c r="D30" s="42"/>
@@ -3248,7 +3124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -4125,7 +4001,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D51D51-DE4C-4B5C-90F6-8EADB68EB458}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0"/>
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -4151,7 +4029,7 @@
       <c r="E1" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="86" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4174,7 +4052,7 @@
         <f>D2/C2%</f>
         <v>0</v>
       </c>
-      <c r="F2" s="86"/>
+      <c r="F2" s="87"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1">
       <c r="A3" s="47">
@@ -4195,7 +4073,7 @@
         <f t="shared" ref="E3:E4" si="0">D3/C3%</f>
         <v>0</v>
       </c>
-      <c r="F3" s="86"/>
+      <c r="F3" s="87"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
       <c r="C4" s="46">

</xml_diff>

<commit_message>
COMIENZO EL MODULO REPORTES EN ADMIN
</commit_message>
<xml_diff>
--- a/assets/PFPL01 - Lista de chequeo producto software.xlsx
+++ b/assets/PFPL01 - Lista de chequeo producto software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\APP-WEB-SENA-2\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9A46BA-5D98-4BC7-851E-B81B078CF6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5724DEF-0CAF-4091-A880-25E6E0F7A570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="772" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="118">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -377,6 +377,30 @@
   </si>
   <si>
     <t>PAGOS</t>
+  </si>
+  <si>
+    <t>inicio de sesion</t>
+  </si>
+  <si>
+    <t>recuperar contraseña</t>
+  </si>
+  <si>
+    <t>crear rol</t>
+  </si>
+  <si>
+    <t>consultar rol</t>
+  </si>
+  <si>
+    <t>modificar rol</t>
+  </si>
+  <si>
+    <t>eliminar rol</t>
+  </si>
+  <si>
+    <t>Registrar usuario</t>
+  </si>
+  <si>
+    <t>consultar usuario</t>
   </si>
 </sst>
 </file>
@@ -1268,28 +1292,44 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1320,42 +1360,26 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1732,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A635BB-A94A-407B-BBB0-F2B3339CC475}">
   <dimension ref="A2:P82"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D26" sqref="D26:E26"/>
     </sheetView>
   </sheetViews>
@@ -1755,91 +1779,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
     </row>
     <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickTop="1">
       <c r="F6" s="10"/>
     </row>
     <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.75" thickTop="1">
       <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="81"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="63"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="69"/>
     </row>
     <row r="13" spans="2:6" ht="18.75" thickBot="1">
       <c r="B13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="63"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="65"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="13" t="s">
         <v>23</v>
       </c>
@@ -1851,10 +1875,10 @@
       <c r="B15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="67"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="15" t="s">
         <v>27</v>
       </c>
@@ -1866,10 +1890,10 @@
       <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="17" t="s">
         <v>30</v>
       </c>
@@ -1879,8 +1903,8 @@
     </row>
     <row r="17" spans="2:16" ht="17.25" thickTop="1">
       <c r="B17" s="19"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -1899,10 +1923,10 @@
       <c r="C21" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="71" t="s">
+      <c r="D21" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="71"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="24" t="s">
         <v>36</v>
       </c>
@@ -1914,10 +1938,10 @@
       <c r="C22" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="72"/>
+      <c r="E22" s="78"/>
       <c r="F22" s="27" t="s">
         <v>24</v>
       </c>
@@ -1925,57 +1949,57 @@
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
       <c r="F23" s="30"/>
     </row>
     <row r="24" spans="2:16" ht="25.5" customHeight="1">
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
       <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -1986,51 +2010,51 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="80" t="s">
+      <c r="B34" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="82"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="63"/>
     </row>
     <row r="35" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="83"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="85"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="66"/>
     </row>
     <row r="36" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="73"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="75"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="55"/>
       <c r="J36" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="73"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="75"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="55"/>
     </row>
     <row r="38" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="73"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="75"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="55"/>
     </row>
     <row r="39" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="76"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="78"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="58"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="34"/>
@@ -2191,16 +2215,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
@@ -2213,12 +2233,16 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2231,8 +2255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2271,7 +2295,9 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="str">
         <f>IF(C3="Cumple","Ninguna","")</f>
@@ -2282,7 +2308,9 @@
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="52"/>
+      <c r="B4" s="52" t="s">
+        <v>111</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6" t="str">
         <f t="shared" ref="D4:D16" si="0">IF(C4="Cumple","Ninguna","")</f>
@@ -2293,7 +2321,9 @@
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="52"/>
+      <c r="B5" s="52" t="s">
+        <v>112</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2304,7 +2334,9 @@
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="52"/>
+      <c r="B6" s="52" t="s">
+        <v>113</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2315,7 +2347,9 @@
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2326,7 +2360,9 @@
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2337,7 +2373,9 @@
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2348,7 +2386,9 @@
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2359,7 +2399,9 @@
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2370,7 +2412,9 @@
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3124,7 +3168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>

</xml_diff>